<commit_message>
'Network+Practical': updated LSTM results, more report written
</commit_message>
<xml_diff>
--- a/02_network_and_practical/src/results/Fine_Tuning_Results.xlsx
+++ b/02_network_and_practical/src/results/Fine_Tuning_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniele\Documents\Programmazione\Github\Uni_NLP2022_Exam\02_network_and_practical\src\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A11E31-7DCA-49E8-B4FB-6F2567DEB335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0BEDA2-294E-4118-BF6B-FB83B89D0A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9495" yWindow="17685" windowWidth="19140" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
     <t>Language</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Swedish</t>
   </si>
   <si>
-    <t>59m</t>
-  </si>
-  <si>
     <t>Batch Size</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t>Long Short Term Memory - Best Hyperparameters</t>
   </si>
   <si>
-    <t>0.0</t>
-  </si>
-  <si>
     <t>Long Short Term Memory - Test Set Results</t>
   </si>
   <si>
@@ -112,12 +106,51 @@
   </si>
   <si>
     <t>Accuracy [2]</t>
+  </si>
+  <si>
+    <t>16h 36m (996m)</t>
+  </si>
+  <si>
+    <t>14h 20m (860m)</t>
+  </si>
+  <si>
+    <t>0h 59m</t>
+  </si>
+  <si>
+    <t>1h 02m</t>
+  </si>
+  <si>
+    <t>0h 54m</t>
+  </si>
+  <si>
+    <t>1m 14s</t>
+  </si>
+  <si>
+    <t>1m 05s</t>
+  </si>
+  <si>
+    <t>Val Accuracy (mean)</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>15h 38m (938m)</t>
+  </si>
+  <si>
+    <t>1m 10s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -144,7 +177,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,8 +214,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -346,24 +385,101 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -372,18 +488,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -425,6 +529,51 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -707,293 +856,418 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:W9"/>
+  <dimension ref="B2:Z9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3" max="5" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="25.7109375" style="10" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="1"/>
     <col min="7" max="7" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8" max="10" width="16.7109375" style="17" customWidth="1"/>
+    <col min="8" max="10" width="16.7109375" style="10" customWidth="1"/>
     <col min="11" max="14" width="16.7109375" style="1" customWidth="1"/>
     <col min="15" max="15" width="22" style="1" customWidth="1"/>
     <col min="16" max="16" width="9.140625" style="1"/>
     <col min="17" max="17" width="12.7109375" style="1" customWidth="1"/>
-    <col min="18" max="20" width="18.7109375" style="17" customWidth="1"/>
+    <col min="18" max="20" width="18.7109375" style="10" customWidth="1"/>
     <col min="21" max="23" width="18.7109375" style="1" customWidth="1"/>
     <col min="24" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:23" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+    <row r="2" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:26" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
+      <c r="G3" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="4"/>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="33"/>
+      <c r="Q3" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="4"/>
-      <c r="Q3" s="2" t="s">
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="32"/>
+      <c r="U3" s="32"/>
+      <c r="V3" s="32"/>
+      <c r="W3" s="33"/>
+    </row>
+    <row r="4" spans="2:26" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="O4" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="S4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="4"/>
+      <c r="T4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="4" spans="2:23" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="5" t="s">
+    <row r="5" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="8">
+        <v>64</v>
+      </c>
+      <c r="I5" s="9">
+        <v>3506</v>
+      </c>
+      <c r="J5" s="9">
+        <v>1024</v>
+      </c>
+      <c r="K5" s="8">
+        <v>2048</v>
+      </c>
+      <c r="L5" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="M5" s="9">
         <v>0</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="N5" s="15">
+        <v>31</v>
+      </c>
+      <c r="O5" s="15">
+        <v>0.8488</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="R5" s="26">
+        <v>0.55610000000000004</v>
+      </c>
+      <c r="S5" s="25">
+        <v>0.82169999999999999</v>
+      </c>
+      <c r="T5" s="25">
+        <v>0.82130000000000003</v>
+      </c>
+      <c r="U5" s="26">
+        <v>0.83069999999999999</v>
+      </c>
+      <c r="V5" s="25">
+        <v>0.84740000000000004</v>
+      </c>
+      <c r="W5" s="25">
+        <v>0.78590000000000004</v>
+      </c>
+      <c r="Y5" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z5" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="11">
+        <v>64</v>
+      </c>
+      <c r="I6" s="12">
+        <v>4216</v>
+      </c>
+      <c r="J6" s="12">
+        <v>1024</v>
+      </c>
+      <c r="K6" s="11">
+        <v>1024</v>
+      </c>
+      <c r="L6" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="M6" s="12">
+        <v>0</v>
+      </c>
+      <c r="N6" s="16">
+        <v>42</v>
+      </c>
+      <c r="O6" s="16">
+        <v>0.77739999999999998</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="R6" s="28">
+        <v>0.92230000000000001</v>
+      </c>
+      <c r="S6" s="27">
+        <v>0.75749999999999995</v>
+      </c>
+      <c r="T6" s="27">
+        <v>0.7601</v>
+      </c>
+      <c r="U6" s="28">
+        <v>0.70250000000000001</v>
+      </c>
+      <c r="V6" s="27">
+        <v>0.76319999999999999</v>
+      </c>
+      <c r="W6" s="27">
+        <v>0.81459999999999999</v>
+      </c>
+      <c r="Y6" s="21">
+        <v>0.6</v>
+      </c>
+      <c r="Z6" s="22">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="7" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="11">
+        <v>64</v>
+      </c>
+      <c r="I7" s="12">
+        <v>4180</v>
+      </c>
+      <c r="J7" s="12">
+        <v>1024</v>
+      </c>
+      <c r="K7" s="11">
+        <v>2048</v>
+      </c>
+      <c r="L7" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="M7" s="12">
+        <v>0</v>
+      </c>
+      <c r="N7" s="16">
+        <v>34</v>
+      </c>
+      <c r="O7" s="16">
+        <v>0.8538</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="R7" s="28">
+        <v>0.54149999999999998</v>
+      </c>
+      <c r="S7" s="27">
+        <v>0.81330000000000002</v>
+      </c>
+      <c r="T7" s="27">
+        <v>0.81379999999999997</v>
+      </c>
+      <c r="U7" s="27">
+        <v>0.80320000000000003</v>
+      </c>
+      <c r="V7" s="28">
+        <v>0.82630000000000003</v>
+      </c>
+      <c r="W7" s="27">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="Y7" s="19">
         <v>1</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="Z7" s="20">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="11">
+        <v>64</v>
+      </c>
+      <c r="I8" s="12">
+        <v>5255</v>
+      </c>
+      <c r="J8" s="12">
+        <v>1024</v>
+      </c>
+      <c r="K8" s="11">
+        <v>1024</v>
+      </c>
+      <c r="L8" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="M8" s="12">
         <v>0</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="6" t="s">
+      <c r="N8" s="16">
         <v>13</v>
       </c>
-      <c r="J4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="N4" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="O4" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="S4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="T4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="U4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="V4" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="W4" s="6" t="s">
-        <v>28</v>
+      <c r="O8" s="16">
+        <v>0.84619999999999995</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R8" s="28">
+        <v>0.6351</v>
+      </c>
+      <c r="S8" s="27">
+        <v>0.8075</v>
+      </c>
+      <c r="T8" s="27">
+        <v>0.80859999999999999</v>
+      </c>
+      <c r="U8" s="28">
+        <v>0.78490000000000004</v>
+      </c>
+      <c r="V8" s="27">
+        <v>0.82369999999999999</v>
+      </c>
+      <c r="W8" s="27">
+        <v>0.81720000000000004</v>
       </c>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="15">
+    <row r="9" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="G9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="13">
         <v>64</v>
       </c>
-      <c r="I5" s="16">
-        <v>3506</v>
-      </c>
-      <c r="J5" s="16">
-        <v>1024</v>
-      </c>
-      <c r="K5" s="15">
-        <v>2048</v>
-      </c>
-      <c r="L5" s="16">
-        <v>1E-3</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="N5" s="22">
-        <v>31</v>
-      </c>
-      <c r="O5" s="22">
-        <v>0.8488</v>
-      </c>
-      <c r="Q5" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="R5" s="15">
-        <v>0.55610000000000004</v>
-      </c>
-      <c r="S5" s="16">
-        <v>0.82169999999999999</v>
-      </c>
-      <c r="T5" s="16">
-        <v>0.82130000000000003</v>
-      </c>
-      <c r="U5" s="15">
-        <v>0.83069999999999999</v>
-      </c>
-      <c r="V5" s="16">
-        <v>0.84740000000000004</v>
-      </c>
-      <c r="W5" s="16">
-        <v>0.78590000000000004</v>
-      </c>
-    </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="G6" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="18"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="Q6" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="R6" s="18"/>
-      <c r="S6" s="19"/>
-      <c r="T6" s="19"/>
-      <c r="U6" s="18"/>
-      <c r="V6" s="19"/>
-      <c r="W6" s="19"/>
-    </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="G7" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="18"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="Q7" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="R7" s="18"/>
-      <c r="S7" s="19"/>
-      <c r="T7" s="19"/>
-      <c r="U7" s="18"/>
-      <c r="V7" s="19"/>
-      <c r="W7" s="19"/>
-    </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B8" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="G8" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="18"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="Q8" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="R8" s="18"/>
-      <c r="S8" s="19"/>
-      <c r="T8" s="19"/>
-      <c r="U8" s="18"/>
-      <c r="V8" s="19"/>
-      <c r="W8" s="19"/>
-    </row>
-    <row r="9" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="14" t="s">
+      <c r="I9" s="14">
+        <v>4010</v>
+      </c>
+      <c r="J9" s="14"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="Q9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="G9" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="20"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="24"/>
-      <c r="O9" s="24"/>
-      <c r="Q9" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="R9" s="20"/>
-      <c r="S9" s="21"/>
-      <c r="T9" s="21"/>
-      <c r="U9" s="20"/>
-      <c r="V9" s="21"/>
-      <c r="W9" s="21"/>
+      <c r="R9" s="30"/>
+      <c r="S9" s="29"/>
+      <c r="T9" s="29"/>
+      <c r="U9" s="30"/>
+      <c r="V9" s="29"/>
+      <c r="W9" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1001,6 +1275,50 @@
     <mergeCell ref="G3:O3"/>
     <mergeCell ref="Q3:W3"/>
   </mergeCells>
+  <conditionalFormatting sqref="S5:W9">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y6:Z6 S5:W9">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R5:R6 Y7:Z7">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R5:R9 Y7:Z7">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
'Network+Practical': obtained all lstm res, revised report
</commit_message>
<xml_diff>
--- a/02_network_and_practical/src/results/Fine_Tuning_Results.xlsx
+++ b/02_network_and_practical/src/results/Fine_Tuning_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniele\Documents\Programmazione\Github\Uni_NLP2022_Exam\02_network_and_practical\src\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0BEDA2-294E-4118-BF6B-FB83B89D0A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37ADDF05-996C-414B-878A-F97389B0EF3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9495" yWindow="17685" windowWidth="19140" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="8220" windowWidth="19140" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
   <si>
     <t>Language</t>
   </si>
@@ -81,15 +81,6 @@
     <t>Dropout</t>
   </si>
   <si>
-    <t>Long Short Term Memory - Training Times</t>
-  </si>
-  <si>
-    <t>Long Short Term Memory - Best Hyperparameters</t>
-  </si>
-  <si>
-    <t>Long Short Term Memory - Test Set Results</t>
-  </si>
-  <si>
     <t>Loss (global)</t>
   </si>
   <si>
@@ -142,6 +133,24 @@
   </si>
   <si>
     <t>1m 10s</t>
+  </si>
+  <si>
+    <t>16h 12m (972m)</t>
+  </si>
+  <si>
+    <t>1h 01m</t>
+  </si>
+  <si>
+    <t>1m 13s</t>
+  </si>
+  <si>
+    <t>[LSTM] Best Hyperparameters, Best Epoch and Val Accuracy</t>
+  </si>
+  <si>
+    <t>[LSTM] Test Set Results</t>
+  </si>
+  <si>
+    <t>[LSTM] Training Times</t>
   </si>
 </sst>
 </file>
@@ -858,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Z9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="W20" sqref="W20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,13 +892,13 @@
     <row r="2" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:26" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="31" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="C3" s="32"/>
       <c r="D3" s="32"/>
       <c r="E3" s="33"/>
       <c r="G3" s="31" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="H3" s="32"/>
       <c r="I3" s="32"/>
@@ -900,7 +909,7 @@
       <c r="N3" s="32"/>
       <c r="O3" s="33"/>
       <c r="Q3" s="31" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="R3" s="32"/>
       <c r="S3" s="32"/>
@@ -947,28 +956,28 @@
         <v>11</v>
       </c>
       <c r="O4" s="18" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="R4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="U4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -979,7 +988,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>13</v>
@@ -1033,10 +1042,10 @@
         <v>0.78590000000000004</v>
       </c>
       <c r="Y5" s="23" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="Z5" s="24" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.25">
@@ -1044,13 +1053,13 @@
         <v>6</v>
       </c>
       <c r="C6" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>30</v>
-      </c>
       <c r="E6" s="12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>6</v>
@@ -1101,7 +1110,7 @@
         <v>0.81459999999999999</v>
       </c>
       <c r="Y6" s="21">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="Z6" s="22">
         <v>0.85</v>
@@ -1112,13 +1121,13 @@
         <v>7</v>
       </c>
       <c r="C7" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>31</v>
-      </c>
       <c r="E7" s="12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>7</v>
@@ -1180,13 +1189,13 @@
         <v>8</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>8</v>
@@ -1241,9 +1250,15 @@
       <c r="B9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
+      <c r="C9" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>38</v>
+      </c>
       <c r="G9" s="7" t="s">
         <v>9</v>
       </c>
@@ -1253,21 +1268,45 @@
       <c r="I9" s="14">
         <v>4010</v>
       </c>
-      <c r="J9" s="14"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
+      <c r="J9" s="14">
+        <v>1024</v>
+      </c>
+      <c r="K9" s="13">
+        <v>1024</v>
+      </c>
+      <c r="L9" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="M9" s="14">
+        <v>0</v>
+      </c>
+      <c r="N9" s="17">
+        <v>48</v>
+      </c>
+      <c r="O9" s="17">
+        <v>0.84589999999999999</v>
+      </c>
       <c r="Q9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="R9" s="30"/>
-      <c r="S9" s="29"/>
-      <c r="T9" s="29"/>
-      <c r="U9" s="30"/>
-      <c r="V9" s="29"/>
-      <c r="W9" s="29"/>
+      <c r="R9" s="30">
+        <v>0.92110000000000003</v>
+      </c>
+      <c r="S9" s="29">
+        <v>0.81920000000000004</v>
+      </c>
+      <c r="T9" s="29">
+        <v>0.8196</v>
+      </c>
+      <c r="U9" s="30">
+        <v>0.81240000000000001</v>
+      </c>
+      <c r="V9" s="29">
+        <v>0.85</v>
+      </c>
+      <c r="W9" s="29">
+        <v>0.79</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
'Network+Practical': implemented LinearSVC + got all results
</commit_message>
<xml_diff>
--- a/02_network_and_practical/src/results/Fine_Tuning_Results.xlsx
+++ b/02_network_and_practical/src/results/Fine_Tuning_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniele\Documents\Programmazione\Github\Uni_NLP2022_Exam\02_network_and_practical\src\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37ADDF05-996C-414B-878A-F97389B0EF3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F4AB87-8931-4FE0-82AA-83D606EBD820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="8220" windowWidth="19140" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="52">
   <si>
     <t>Language</t>
   </si>
@@ -151,14 +151,45 @@
   </si>
   <si>
     <t>[LSTM] Training Times</t>
+  </si>
+  <si>
+    <t>[CNN] Training Times</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>2m 43s</t>
+  </si>
+  <si>
+    <t>5s</t>
+  </si>
+  <si>
+    <t>[LSVC] Best C and Val Accuracy</t>
+  </si>
+  <si>
+    <t>[LSVC] Training Times</t>
+  </si>
+  <si>
+    <t>[LSVC] Test Set Results</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>[CNN] Best Hyperparameters, Best Epoch and Val Accuracy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -186,7 +217,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -229,8 +260,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCA83F5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCD6F5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -480,11 +535,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -583,6 +653,69 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -591,6 +724,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFCD6F5"/>
+      <color rgb="FFCA83F5"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -865,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Z9"/>
+  <dimension ref="B2:Z41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="W20" sqref="W20"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="T32" sqref="T32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,7 +1029,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:26" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:26" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="31" t="s">
         <v>41</v>
       </c>
@@ -1110,10 +1249,10 @@
         <v>0.81459999999999999</v>
       </c>
       <c r="Y6" s="21">
-        <v>0.5</v>
+        <v>0.65</v>
       </c>
       <c r="Z6" s="22">
-        <v>0.85</v>
+        <v>0.91500000000000004</v>
       </c>
     </row>
     <row r="7" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1308,13 +1447,638 @@
         <v>0.79</v>
       </c>
     </row>
+    <row r="10" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="2:26" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="36"/>
+      <c r="G11" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="35"/>
+      <c r="N11" s="35"/>
+      <c r="O11" s="36"/>
+      <c r="Q11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="R11" s="35"/>
+      <c r="S11" s="35"/>
+      <c r="T11" s="35"/>
+      <c r="U11" s="35"/>
+      <c r="V11" s="35"/>
+      <c r="W11" s="36"/>
+    </row>
+    <row r="12" spans="2:26" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="44"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="44"/>
+      <c r="L12" s="44"/>
+      <c r="M12" s="45"/>
+      <c r="N12" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="O12" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q12" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="R12" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="S12" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="T12" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="U12" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="V12" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="W12" s="44" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="G13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="8"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="Q13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="R13" s="26"/>
+      <c r="S13" s="25"/>
+      <c r="T13" s="25"/>
+      <c r="U13" s="26"/>
+      <c r="V13" s="25"/>
+      <c r="W13" s="25"/>
+    </row>
+    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="G14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="11"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="Q14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="R14" s="28"/>
+      <c r="S14" s="27"/>
+      <c r="T14" s="27"/>
+      <c r="U14" s="28"/>
+      <c r="V14" s="27"/>
+      <c r="W14" s="27"/>
+    </row>
+    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="G15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="11"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="Q15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="R15" s="28"/>
+      <c r="S15" s="27"/>
+      <c r="T15" s="27"/>
+      <c r="U15" s="27"/>
+      <c r="V15" s="28"/>
+      <c r="W15" s="27"/>
+    </row>
+    <row r="16" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="G16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="11"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="Q16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R16" s="28"/>
+      <c r="S16" s="27"/>
+      <c r="T16" s="27"/>
+      <c r="U16" s="28"/>
+      <c r="V16" s="27"/>
+      <c r="W16" s="27"/>
+    </row>
+    <row r="17" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="G17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="13"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="Q17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="R17" s="30"/>
+      <c r="S17" s="29"/>
+      <c r="T17" s="29"/>
+      <c r="U17" s="30"/>
+      <c r="V17" s="29"/>
+      <c r="W17" s="29"/>
+    </row>
+    <row r="18" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="2:23" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="51"/>
+      <c r="D19" s="52"/>
+      <c r="G19" s="10"/>
+      <c r="J19" s="1"/>
+      <c r="M19" s="50" t="s">
+        <v>47</v>
+      </c>
+      <c r="N19" s="51"/>
+      <c r="O19" s="52"/>
+      <c r="Q19" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="R19" s="51"/>
+      <c r="S19" s="51"/>
+      <c r="T19" s="51"/>
+      <c r="U19" s="51"/>
+      <c r="V19" s="51"/>
+      <c r="W19" s="52"/>
+    </row>
+    <row r="20" spans="2:23" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="54" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" s="10"/>
+      <c r="J20" s="1"/>
+      <c r="M20" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="N20" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="O20" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q20" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="R20" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="S20" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="T20" s="54" t="s">
+        <v>20</v>
+      </c>
+      <c r="U20" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="V20" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="W20" s="54" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G21" s="10"/>
+      <c r="J21" s="1"/>
+      <c r="M21" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="N21" s="37">
+        <v>1</v>
+      </c>
+      <c r="O21" s="40">
+        <v>0.91120000000000001</v>
+      </c>
+      <c r="Q21" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="R21" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="S21" s="25">
+        <v>0.87919999999999998</v>
+      </c>
+      <c r="T21" s="25">
+        <v>0.87829999999999997</v>
+      </c>
+      <c r="U21" s="26">
+        <v>0.90780000000000005</v>
+      </c>
+      <c r="V21" s="25">
+        <v>0.86009999999999998</v>
+      </c>
+      <c r="W21" s="25">
+        <v>0.86699999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="G22" s="10"/>
+      <c r="J22" s="1"/>
+      <c r="M22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="N22" s="38">
+        <v>1</v>
+      </c>
+      <c r="O22" s="41">
+        <v>0.91214200000000001</v>
+      </c>
+      <c r="Q22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="R22" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="S22" s="27">
+        <v>0.87580000000000002</v>
+      </c>
+      <c r="T22" s="27">
+        <v>0.875</v>
+      </c>
+      <c r="U22" s="28">
+        <v>0.91169999999999995</v>
+      </c>
+      <c r="V22" s="27">
+        <v>0.85940000000000005</v>
+      </c>
+      <c r="W22" s="27">
+        <v>0.85389999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="G23" s="10"/>
+      <c r="J23" s="1"/>
+      <c r="M23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N23" s="38">
+        <v>1</v>
+      </c>
+      <c r="O23" s="41">
+        <v>0.90961499999999995</v>
+      </c>
+      <c r="Q23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="R23" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="S23" s="27">
+        <v>0.87749999999999995</v>
+      </c>
+      <c r="T23" s="27">
+        <v>0.87680000000000002</v>
+      </c>
+      <c r="U23" s="27">
+        <v>0.90739999999999998</v>
+      </c>
+      <c r="V23" s="28">
+        <v>0.8528</v>
+      </c>
+      <c r="W23" s="27">
+        <v>0.87009999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="G24" s="10"/>
+      <c r="J24" s="1"/>
+      <c r="M24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="N24" s="38">
+        <v>1</v>
+      </c>
+      <c r="O24" s="41">
+        <v>0.91226200000000002</v>
+      </c>
+      <c r="Q24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R24" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="S24" s="27">
+        <v>0.88</v>
+      </c>
+      <c r="T24" s="27">
+        <v>0.87919999999999998</v>
+      </c>
+      <c r="U24" s="28">
+        <v>0.91410000000000002</v>
+      </c>
+      <c r="V24" s="27">
+        <v>0.86680000000000001</v>
+      </c>
+      <c r="W24" s="27">
+        <v>0.85680000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G25" s="10"/>
+      <c r="J25" s="1"/>
+      <c r="M25" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="N25" s="39">
+        <v>1</v>
+      </c>
+      <c r="O25" s="42">
+        <v>0.90903299999999998</v>
+      </c>
+      <c r="Q25" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="R25" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="S25" s="29">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="T25" s="29">
+        <v>0.88419999999999999</v>
+      </c>
+      <c r="U25" s="30">
+        <v>0.91249999999999998</v>
+      </c>
+      <c r="V25" s="29">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="W25" s="29">
+        <v>0.88109999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="G26" s="10"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="G27" s="10"/>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="G28" s="10"/>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="G29" s="10"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="36" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G36" s="10"/>
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G37" s="10"/>
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G38" s="10"/>
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G39" s="10"/>
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G40" s="10"/>
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G41" s="10"/>
+      <c r="J41" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="9">
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="G3:O3"/>
     <mergeCell ref="Q3:W3"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="G11:O11"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="Q19:W19"/>
+    <mergeCell ref="Q11:W11"/>
   </mergeCells>
   <conditionalFormatting sqref="S5:W9">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y6:Z6 S5:W9">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R5:R6 Y7:Z7">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R5:R9 Y7:Z7">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S21:W25">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S21:W25">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R21:R24">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R21:R25">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S5:W9 S21:W25 Y6:Z6">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S13:W17">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S13:W17">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -1326,8 +2090,28 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y6:Z6 S5:W9">
+  <conditionalFormatting sqref="R13:R14">
     <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R13:R17">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S13:W17">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1338,26 +2122,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R5:R6 Y7:Z7">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R5:R9 Y7:Z7">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Implemented grid search for CNN, obtained en results
</commit_message>
<xml_diff>
--- a/02_network_and_practical/src/results/Fine_Tuning_Results.xlsx
+++ b/02_network_and_practical/src/results/Fine_Tuning_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniele\Documents\Programmazione\Github\Uni_NLP2022_Exam\02_network_and_practical\src\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B6F143-AF52-4703-9A90-8A50743A41F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A28B1C-0B7C-4860-B598-CF92AA823132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9015" yWindow="13125" windowWidth="19140" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="59">
   <si>
     <t>Language</t>
   </si>
@@ -162,9 +162,6 @@
     <t>C</t>
   </si>
   <si>
-    <t>2m 43s</t>
-  </si>
-  <si>
     <t>5s</t>
   </si>
   <si>
@@ -181,6 +178,30 @@
   </si>
   <si>
     <t>[CNN] Best Hyperparameters, Best Epoch and Val Accuracy</t>
+  </si>
+  <si>
+    <t>2h 06m</t>
+  </si>
+  <si>
+    <t>1m 19s</t>
+  </si>
+  <si>
+    <t>1.6s</t>
+  </si>
+  <si>
+    <t>Kernel Size</t>
+  </si>
+  <si>
+    <t>Stride</t>
+  </si>
+  <si>
+    <t>Padding</t>
+  </si>
+  <si>
+    <t>[CNN] Test Set Results</t>
+  </si>
+  <si>
+    <t>2m 43s (on CPU)</t>
   </si>
 </sst>
 </file>
@@ -1004,9 +1025,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Z41"/>
+  <dimension ref="B2:AB41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -1014,50 +1035,51 @@
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="25.7109375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="23.7109375" style="10" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="1"/>
-    <col min="7" max="7" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8" max="10" width="16.7109375" style="10" customWidth="1"/>
-    <col min="11" max="14" width="16.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="22" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" style="1"/>
-    <col min="17" max="17" width="12.7109375" style="1" customWidth="1"/>
-    <col min="18" max="20" width="18.7109375" style="10" customWidth="1"/>
-    <col min="21" max="23" width="18.7109375" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="16.7109375" style="1" customWidth="1"/>
+    <col min="8" max="12" width="16.7109375" style="10" customWidth="1"/>
+    <col min="13" max="16" width="16.7109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="22.140625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" style="1"/>
+    <col min="19" max="19" width="12.7109375" style="1" customWidth="1"/>
+    <col min="20" max="22" width="18.7109375" style="10" customWidth="1"/>
+    <col min="23" max="25" width="18.7109375" style="1" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:26" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:28" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="46" t="s">
         <v>41</v>
       </c>
       <c r="C3" s="47"/>
       <c r="D3" s="47"/>
       <c r="E3" s="48"/>
-      <c r="G3" s="46" t="s">
+      <c r="G3" s="10"/>
+      <c r="I3" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
       <c r="J3" s="47"/>
       <c r="K3" s="47"/>
       <c r="L3" s="47"/>
       <c r="M3" s="47"/>
       <c r="N3" s="47"/>
-      <c r="O3" s="48"/>
-      <c r="Q3" s="46" t="s">
+      <c r="O3" s="47"/>
+      <c r="P3" s="47"/>
+      <c r="Q3" s="48"/>
+      <c r="S3" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="R3" s="47"/>
-      <c r="S3" s="47"/>
       <c r="T3" s="47"/>
       <c r="U3" s="47"/>
       <c r="V3" s="47"/>
-      <c r="W3" s="48"/>
-    </row>
-    <row r="4" spans="2:26" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W3" s="47"/>
+      <c r="X3" s="47"/>
+      <c r="Y3" s="48"/>
+    </row>
+    <row r="4" spans="2:28" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1070,56 +1092,57 @@
       <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="10"/>
+      <c r="I4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="18" t="s">
+      <c r="P4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="18" t="s">
+      <c r="Q4" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="S4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="X4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
@@ -1132,62 +1155,63 @@
       <c r="E5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="10"/>
+      <c r="I5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="8">
+      <c r="J5" s="8">
         <v>64</v>
       </c>
-      <c r="I5" s="9">
+      <c r="K5" s="9">
         <v>3506</v>
       </c>
-      <c r="J5" s="9">
+      <c r="L5" s="9">
         <v>1024</v>
       </c>
-      <c r="K5" s="8">
+      <c r="M5" s="8">
         <v>2048</v>
       </c>
-      <c r="L5" s="9">
+      <c r="N5" s="9">
         <v>1E-3</v>
       </c>
-      <c r="M5" s="9">
+      <c r="O5" s="9">
         <v>0</v>
       </c>
-      <c r="N5" s="15">
+      <c r="P5" s="15">
         <v>31</v>
       </c>
-      <c r="O5" s="15">
+      <c r="Q5" s="15">
         <v>0.8488</v>
       </c>
-      <c r="Q5" s="5" t="s">
+      <c r="S5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="R5" s="26">
+      <c r="T5" s="26">
         <v>0.55610000000000004</v>
       </c>
-      <c r="S5" s="25">
+      <c r="U5" s="25">
         <v>0.82169999999999999</v>
       </c>
-      <c r="T5" s="25">
+      <c r="V5" s="25">
         <v>0.82130000000000003</v>
       </c>
-      <c r="U5" s="26">
+      <c r="W5" s="26">
         <v>0.83069999999999999</v>
       </c>
-      <c r="V5" s="25">
+      <c r="X5" s="25">
         <v>0.84740000000000004</v>
       </c>
-      <c r="W5" s="25">
+      <c r="Y5" s="25">
         <v>0.78590000000000004</v>
       </c>
-      <c r="Y5" s="23" t="s">
+      <c r="AA5" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="Z5" s="24" t="s">
+      <c r="AB5" s="24" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
@@ -1200,62 +1224,63 @@
       <c r="E6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="10"/>
+      <c r="I6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="11">
+      <c r="J6" s="11">
         <v>64</v>
       </c>
-      <c r="I6" s="12">
+      <c r="K6" s="12">
         <v>4216</v>
       </c>
-      <c r="J6" s="12">
+      <c r="L6" s="12">
         <v>1024</v>
       </c>
-      <c r="K6" s="11">
+      <c r="M6" s="11">
         <v>1024</v>
       </c>
-      <c r="L6" s="12">
+      <c r="N6" s="12">
         <v>1E-3</v>
       </c>
-      <c r="M6" s="12">
+      <c r="O6" s="12">
         <v>0</v>
       </c>
-      <c r="N6" s="16">
+      <c r="P6" s="16">
         <v>42</v>
       </c>
-      <c r="O6" s="16">
+      <c r="Q6" s="16">
         <v>0.77739999999999998</v>
       </c>
-      <c r="Q6" s="6" t="s">
+      <c r="S6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="R6" s="28">
+      <c r="T6" s="28">
         <v>0.92230000000000001</v>
       </c>
-      <c r="S6" s="27">
+      <c r="U6" s="27">
         <v>0.75749999999999995</v>
       </c>
-      <c r="T6" s="27">
+      <c r="V6" s="27">
         <v>0.7601</v>
       </c>
-      <c r="U6" s="28">
+      <c r="W6" s="28">
         <v>0.70250000000000001</v>
       </c>
-      <c r="V6" s="27">
+      <c r="X6" s="27">
         <v>0.76319999999999999</v>
       </c>
-      <c r="W6" s="27">
+      <c r="Y6" s="27">
         <v>0.81459999999999999</v>
       </c>
-      <c r="Y6" s="21">
+      <c r="AA6" s="21">
         <v>0.65</v>
       </c>
-      <c r="Z6" s="22">
+      <c r="AB6" s="22">
         <v>0.91500000000000004</v>
       </c>
     </row>
-    <row r="7" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
@@ -1268,62 +1293,63 @@
       <c r="E7" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="10"/>
+      <c r="I7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="11">
+      <c r="J7" s="11">
         <v>64</v>
       </c>
-      <c r="I7" s="12">
+      <c r="K7" s="12">
         <v>4180</v>
       </c>
-      <c r="J7" s="12">
+      <c r="L7" s="12">
         <v>1024</v>
       </c>
-      <c r="K7" s="11">
+      <c r="M7" s="11">
         <v>2048</v>
       </c>
-      <c r="L7" s="12">
+      <c r="N7" s="12">
         <v>1E-3</v>
       </c>
-      <c r="M7" s="12">
+      <c r="O7" s="12">
         <v>0</v>
       </c>
-      <c r="N7" s="16">
+      <c r="P7" s="16">
         <v>34</v>
       </c>
-      <c r="O7" s="16">
+      <c r="Q7" s="16">
         <v>0.8538</v>
       </c>
-      <c r="Q7" s="6" t="s">
+      <c r="S7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="R7" s="28">
+      <c r="T7" s="28">
         <v>0.54149999999999998</v>
       </c>
-      <c r="S7" s="27">
+      <c r="U7" s="27">
         <v>0.81330000000000002</v>
       </c>
-      <c r="T7" s="27">
+      <c r="V7" s="27">
         <v>0.81379999999999997</v>
       </c>
-      <c r="U7" s="27">
+      <c r="W7" s="27">
         <v>0.80320000000000003</v>
       </c>
-      <c r="V7" s="28">
+      <c r="X7" s="28">
         <v>0.82630000000000003</v>
       </c>
-      <c r="W7" s="27">
+      <c r="Y7" s="27">
         <v>0.81200000000000006</v>
       </c>
-      <c r="Y7" s="19">
+      <c r="AA7" s="19">
         <v>1</v>
       </c>
-      <c r="Z7" s="20">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="AB7" s="20">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="8" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
@@ -1336,56 +1362,57 @@
       <c r="E8" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="10"/>
+      <c r="I8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="11">
+      <c r="J8" s="11">
         <v>64</v>
       </c>
-      <c r="I8" s="12">
+      <c r="K8" s="12">
         <v>5255</v>
       </c>
-      <c r="J8" s="12">
+      <c r="L8" s="12">
         <v>1024</v>
       </c>
-      <c r="K8" s="11">
+      <c r="M8" s="11">
         <v>1024</v>
       </c>
-      <c r="L8" s="12">
+      <c r="N8" s="12">
         <v>1E-3</v>
       </c>
-      <c r="M8" s="12">
+      <c r="O8" s="12">
         <v>0</v>
       </c>
-      <c r="N8" s="16">
+      <c r="P8" s="16">
         <v>13</v>
       </c>
-      <c r="O8" s="16">
+      <c r="Q8" s="16">
         <v>0.84619999999999995</v>
       </c>
-      <c r="Q8" s="6" t="s">
+      <c r="S8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="R8" s="28">
+      <c r="T8" s="28">
         <v>0.6351</v>
       </c>
-      <c r="S8" s="27">
+      <c r="U8" s="27">
         <v>0.8075</v>
       </c>
-      <c r="T8" s="27">
+      <c r="V8" s="27">
         <v>0.80859999999999999</v>
       </c>
-      <c r="U8" s="28">
+      <c r="W8" s="28">
         <v>0.78490000000000004</v>
       </c>
-      <c r="V8" s="27">
+      <c r="X8" s="27">
         <v>0.82369999999999999</v>
       </c>
-      <c r="W8" s="27">
+      <c r="Y8" s="27">
         <v>0.81720000000000004</v>
       </c>
     </row>
-    <row r="9" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="7" t="s">
         <v>9</v>
       </c>
@@ -1398,57 +1425,57 @@
       <c r="E9" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="I9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="13">
+      <c r="J9" s="13">
         <v>64</v>
       </c>
-      <c r="I9" s="14">
+      <c r="K9" s="14">
         <v>4010</v>
       </c>
-      <c r="J9" s="14">
+      <c r="L9" s="14">
         <v>1024</v>
       </c>
-      <c r="K9" s="13">
+      <c r="M9" s="13">
         <v>1024</v>
       </c>
-      <c r="L9" s="14">
+      <c r="N9" s="14">
         <v>1E-3</v>
       </c>
-      <c r="M9" s="14">
+      <c r="O9" s="14">
         <v>0</v>
       </c>
-      <c r="N9" s="17">
+      <c r="P9" s="17">
         <v>48</v>
       </c>
-      <c r="O9" s="17">
+      <c r="Q9" s="17">
         <v>0.84589999999999999</v>
       </c>
-      <c r="Q9" s="7" t="s">
+      <c r="S9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="R9" s="30">
+      <c r="T9" s="30">
         <v>0.92110000000000003</v>
       </c>
-      <c r="S9" s="29">
+      <c r="U9" s="29">
         <v>0.81920000000000004</v>
       </c>
-      <c r="T9" s="29">
+      <c r="V9" s="29">
         <v>0.8196</v>
       </c>
-      <c r="U9" s="30">
+      <c r="W9" s="30">
         <v>0.81240000000000001</v>
       </c>
-      <c r="V9" s="29">
+      <c r="X9" s="29">
         <v>0.85</v>
       </c>
-      <c r="W9" s="29">
+      <c r="Y9" s="29">
         <v>0.79</v>
       </c>
     </row>
-    <row r="10" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="2:26" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="2:28" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="49" t="s">
         <v>42</v>
       </c>
@@ -1456,7 +1483,7 @@
       <c r="D11" s="50"/>
       <c r="E11" s="51"/>
       <c r="G11" s="49" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H11" s="50"/>
       <c r="I11" s="50"/>
@@ -1465,18 +1492,20 @@
       <c r="L11" s="50"/>
       <c r="M11" s="50"/>
       <c r="N11" s="50"/>
-      <c r="O11" s="51"/>
-      <c r="Q11" s="49" t="s">
-        <v>40</v>
-      </c>
-      <c r="R11" s="50"/>
-      <c r="S11" s="50"/>
+      <c r="O11" s="50"/>
+      <c r="P11" s="50"/>
+      <c r="Q11" s="51"/>
+      <c r="S11" s="49" t="s">
+        <v>57</v>
+      </c>
       <c r="T11" s="50"/>
       <c r="U11" s="50"/>
       <c r="V11" s="50"/>
-      <c r="W11" s="51"/>
-    </row>
-    <row r="12" spans="2:26" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W11" s="50"/>
+      <c r="X11" s="50"/>
+      <c r="Y11" s="51"/>
+    </row>
+    <row r="12" spans="2:28" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="37" t="s">
         <v>0</v>
       </c>
@@ -1495,68 +1524,124 @@
       <c r="H12" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="38"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="18" t="s">
+      <c r="I12" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="L12" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="M12" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="N12" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="O12" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="P12" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="O12" s="18" t="s">
+      <c r="Q12" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="Q12" s="37" t="s">
+      <c r="S12" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="R12" s="38" t="s">
+      <c r="T12" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="S12" s="38" t="s">
+      <c r="U12" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="T12" s="38" t="s">
+      <c r="V12" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="U12" s="38" t="s">
+      <c r="W12" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="V12" s="38" t="s">
+      <c r="X12" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="W12" s="38" t="s">
+      <c r="Y12" s="38" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
+      <c r="C13" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="G13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="8"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="Q13" s="5" t="s">
+      <c r="H13" s="8">
+        <v>64</v>
+      </c>
+      <c r="I13" s="9">
+        <v>3506</v>
+      </c>
+      <c r="J13" s="9">
+        <v>1024</v>
+      </c>
+      <c r="K13" s="8">
+        <v>5</v>
+      </c>
+      <c r="L13" s="8">
+        <v>1</v>
+      </c>
+      <c r="M13" s="8">
+        <v>3</v>
+      </c>
+      <c r="N13" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="O13" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="P13" s="15">
+        <v>46</v>
+      </c>
+      <c r="Q13" s="15">
+        <v>0.88739999999999997</v>
+      </c>
+      <c r="S13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="R13" s="26"/>
-      <c r="S13" s="25"/>
-      <c r="T13" s="25"/>
-      <c r="U13" s="26"/>
-      <c r="V13" s="25"/>
-      <c r="W13" s="25"/>
-    </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="T13" s="26">
+        <v>0.70850000000000002</v>
+      </c>
+      <c r="U13" s="25">
+        <v>0.84250000000000003</v>
+      </c>
+      <c r="V13" s="25">
+        <v>0.84150000000000003</v>
+      </c>
+      <c r="W13" s="26">
+        <v>0.86270000000000002</v>
+      </c>
+      <c r="X13" s="25">
+        <v>0.82369999999999999</v>
+      </c>
+      <c r="Y13" s="25">
+        <v>0.83809999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
         <v>6</v>
       </c>
@@ -1566,25 +1651,31 @@
       <c r="G14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="12"/>
+      <c r="H14" s="11">
+        <v>64</v>
+      </c>
+      <c r="I14" s="12">
+        <v>4216</v>
+      </c>
       <c r="J14" s="12"/>
       <c r="K14" s="11"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
-      <c r="Q14" s="6" t="s">
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="S14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="R14" s="28"/>
-      <c r="S14" s="27"/>
-      <c r="T14" s="27"/>
-      <c r="U14" s="28"/>
+      <c r="T14" s="28"/>
+      <c r="U14" s="27"/>
       <c r="V14" s="27"/>
-      <c r="W14" s="27"/>
-    </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="W14" s="28"/>
+      <c r="X14" s="27"/>
+      <c r="Y14" s="27"/>
+    </row>
+    <row r="15" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
         <v>7</v>
       </c>
@@ -1594,25 +1685,31 @@
       <c r="G15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H15" s="11"/>
-      <c r="I15" s="12"/>
+      <c r="H15" s="11">
+        <v>64</v>
+      </c>
+      <c r="I15" s="12">
+        <v>4180</v>
+      </c>
       <c r="J15" s="12"/>
       <c r="K15" s="11"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
-      <c r="Q15" s="6" t="s">
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
+      <c r="S15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="R15" s="28"/>
-      <c r="S15" s="27"/>
-      <c r="T15" s="27"/>
+      <c r="T15" s="28"/>
       <c r="U15" s="27"/>
-      <c r="V15" s="28"/>
+      <c r="V15" s="27"/>
       <c r="W15" s="27"/>
-    </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="X15" s="28"/>
+      <c r="Y15" s="27"/>
+    </row>
+    <row r="16" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>8</v>
       </c>
@@ -1622,25 +1719,31 @@
       <c r="G16" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H16" s="11"/>
-      <c r="I16" s="12"/>
+      <c r="H16" s="11">
+        <v>64</v>
+      </c>
+      <c r="I16" s="12">
+        <v>5255</v>
+      </c>
       <c r="J16" s="12"/>
       <c r="K16" s="11"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="16"/>
-      <c r="O16" s="16"/>
-      <c r="Q16" s="6" t="s">
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="S16" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="R16" s="28"/>
-      <c r="S16" s="27"/>
-      <c r="T16" s="27"/>
-      <c r="U16" s="28"/>
+      <c r="T16" s="28"/>
+      <c r="U16" s="27"/>
       <c r="V16" s="27"/>
-      <c r="W16" s="27"/>
-    </row>
-    <row r="17" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W16" s="28"/>
+      <c r="X16" s="27"/>
+      <c r="Y16" s="27"/>
+    </row>
+    <row r="17" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="7" t="s">
         <v>9</v>
       </c>
@@ -1650,49 +1753,57 @@
       <c r="G17" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H17" s="13"/>
-      <c r="I17" s="14"/>
+      <c r="H17" s="13">
+        <v>64</v>
+      </c>
+      <c r="I17" s="14">
+        <v>4010</v>
+      </c>
       <c r="J17" s="14"/>
       <c r="K17" s="13"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="Q17" s="7" t="s">
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="S17" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="R17" s="30"/>
-      <c r="S17" s="29"/>
-      <c r="T17" s="29"/>
-      <c r="U17" s="30"/>
+      <c r="T17" s="30"/>
+      <c r="U17" s="29"/>
       <c r="V17" s="29"/>
-      <c r="W17" s="29"/>
-    </row>
-    <row r="18" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="2:23" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W17" s="30"/>
+      <c r="X17" s="29"/>
+      <c r="Y17" s="29"/>
+    </row>
+    <row r="18" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="2:25" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="52" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" s="53"/>
       <c r="D19" s="54"/>
       <c r="G19" s="10"/>
       <c r="J19" s="1"/>
-      <c r="M19" s="52" t="s">
-        <v>47</v>
-      </c>
-      <c r="N19" s="53"/>
-      <c r="O19" s="54"/>
-      <c r="Q19" s="52" t="s">
-        <v>49</v>
-      </c>
-      <c r="R19" s="53"/>
-      <c r="S19" s="53"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="O19" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="P19" s="53"/>
+      <c r="Q19" s="54"/>
+      <c r="S19" s="52" t="s">
+        <v>48</v>
+      </c>
       <c r="T19" s="53"/>
       <c r="U19" s="53"/>
       <c r="V19" s="53"/>
-      <c r="W19" s="54"/>
-    </row>
-    <row r="20" spans="2:23" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W19" s="53"/>
+      <c r="X19" s="53"/>
+      <c r="Y19" s="54"/>
+    </row>
+    <row r="20" spans="2:25" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="44" t="s">
         <v>0</v>
       </c>
@@ -1704,270 +1815,293 @@
       </c>
       <c r="G20" s="10"/>
       <c r="J20" s="1"/>
-      <c r="M20" s="44" t="s">
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="O20" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="N20" s="45" t="s">
+      <c r="P20" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="O20" s="40" t="s">
+      <c r="Q20" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="Q20" s="44" t="s">
+      <c r="S20" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="R20" s="45" t="s">
+      <c r="T20" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="S20" s="45" t="s">
+      <c r="U20" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="T20" s="45" t="s">
+      <c r="V20" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="U20" s="45" t="s">
+      <c r="W20" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="V20" s="45" t="s">
+      <c r="X20" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="W20" s="45" t="s">
+      <c r="Y20" s="45" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="s">
         <v>43</v>
       </c>
       <c r="C21" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G21" s="10"/>
-      <c r="J21" s="1"/>
-      <c r="M21" s="5" t="s">
+      <c r="L21" s="1"/>
+      <c r="O21" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="N21" s="31">
+      <c r="P21" s="31">
         <v>1</v>
       </c>
-      <c r="O21" s="34">
+      <c r="Q21" s="34">
         <v>0.91120000000000001</v>
       </c>
-      <c r="Q21" s="5" t="s">
+      <c r="S21" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="R21" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="S21" s="25">
+      <c r="T21" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="U21" s="25">
         <v>0.87919999999999998</v>
       </c>
-      <c r="T21" s="25">
+      <c r="V21" s="25">
         <v>0.87829999999999997</v>
       </c>
-      <c r="U21" s="26">
+      <c r="W21" s="26">
         <v>0.90780000000000005</v>
       </c>
-      <c r="V21" s="25">
+      <c r="X21" s="25">
         <v>0.86009999999999998</v>
       </c>
-      <c r="W21" s="25">
+      <c r="Y21" s="25">
         <v>0.86699999999999999</v>
       </c>
     </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="G22" s="10"/>
-      <c r="J22" s="1"/>
-      <c r="M22" s="6" t="s">
+    <row r="22" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="L22" s="1"/>
+      <c r="O22" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="N22" s="32">
+      <c r="P22" s="32">
         <v>1</v>
       </c>
-      <c r="O22" s="35">
+      <c r="Q22" s="35">
         <v>0.91214200000000001</v>
       </c>
-      <c r="Q22" s="6" t="s">
+      <c r="S22" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="R22" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="S22" s="27">
+      <c r="T22" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="U22" s="27">
         <v>0.87580000000000002</v>
       </c>
-      <c r="T22" s="27">
+      <c r="V22" s="27">
         <v>0.875</v>
       </c>
-      <c r="U22" s="28">
+      <c r="W22" s="28">
         <v>0.91169999999999995</v>
       </c>
-      <c r="V22" s="27">
+      <c r="X22" s="27">
         <v>0.85940000000000005</v>
       </c>
-      <c r="W22" s="27">
+      <c r="Y22" s="27">
         <v>0.85389999999999999</v>
       </c>
     </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:25" x14ac:dyDescent="0.25">
       <c r="G23" s="10"/>
       <c r="J23" s="1"/>
-      <c r="M23" s="6" t="s">
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="O23" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N23" s="32">
+      <c r="P23" s="32">
         <v>1</v>
       </c>
-      <c r="O23" s="35">
+      <c r="Q23" s="35">
         <v>0.90961499999999995</v>
       </c>
-      <c r="Q23" s="6" t="s">
+      <c r="S23" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="R23" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="S23" s="27">
+      <c r="T23" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="U23" s="27">
         <v>0.87749999999999995</v>
       </c>
-      <c r="T23" s="27">
+      <c r="V23" s="27">
         <v>0.87680000000000002</v>
       </c>
-      <c r="U23" s="27">
+      <c r="W23" s="27">
         <v>0.90739999999999998</v>
       </c>
-      <c r="V23" s="28">
+      <c r="X23" s="28">
         <v>0.8528</v>
       </c>
-      <c r="W23" s="27">
+      <c r="Y23" s="27">
         <v>0.87009999999999998</v>
       </c>
     </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:25" x14ac:dyDescent="0.25">
       <c r="G24" s="10"/>
       <c r="J24" s="1"/>
-      <c r="M24" s="6" t="s">
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="O24" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N24" s="32">
+      <c r="P24" s="32">
         <v>1</v>
       </c>
-      <c r="O24" s="35">
+      <c r="Q24" s="35">
         <v>0.91226200000000002</v>
       </c>
-      <c r="Q24" s="6" t="s">
+      <c r="S24" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="R24" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="S24" s="27">
+      <c r="T24" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="U24" s="27">
         <v>0.88</v>
       </c>
-      <c r="T24" s="27">
+      <c r="V24" s="27">
         <v>0.87919999999999998</v>
       </c>
-      <c r="U24" s="28">
+      <c r="W24" s="28">
         <v>0.91410000000000002</v>
       </c>
-      <c r="V24" s="27">
+      <c r="X24" s="27">
         <v>0.86680000000000001</v>
       </c>
-      <c r="W24" s="27">
+      <c r="Y24" s="27">
         <v>0.85680000000000001</v>
       </c>
     </row>
-    <row r="25" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G25" s="10"/>
       <c r="J25" s="1"/>
-      <c r="M25" s="7" t="s">
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="O25" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="N25" s="33">
+      <c r="P25" s="33">
         <v>1</v>
       </c>
-      <c r="O25" s="36">
+      <c r="Q25" s="36">
         <v>0.90903299999999998</v>
       </c>
-      <c r="Q25" s="7" t="s">
+      <c r="S25" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="R25" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="S25" s="29">
+      <c r="T25" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="U25" s="29">
         <v>0.88500000000000001</v>
       </c>
-      <c r="T25" s="29">
+      <c r="V25" s="29">
         <v>0.88419999999999999</v>
       </c>
-      <c r="U25" s="30">
+      <c r="W25" s="30">
         <v>0.91249999999999998</v>
       </c>
-      <c r="V25" s="29">
+      <c r="X25" s="29">
         <v>0.85899999999999999</v>
       </c>
-      <c r="W25" s="29">
+      <c r="Y25" s="29">
         <v>0.88109999999999999</v>
       </c>
     </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:25" x14ac:dyDescent="0.25">
       <c r="G26" s="10"/>
       <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+    </row>
+    <row r="27" spans="2:25" x14ac:dyDescent="0.25">
       <c r="G27" s="10"/>
       <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+    </row>
+    <row r="28" spans="2:25" x14ac:dyDescent="0.25">
       <c r="G28" s="10"/>
       <c r="J28" s="1"/>
-    </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="G29" s="10"/>
-      <c r="J29" s="1"/>
-    </row>
-    <row r="36" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+    </row>
+    <row r="29" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="L29" s="1"/>
+    </row>
+    <row r="36" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G36" s="10"/>
       <c r="J36" s="1"/>
-    </row>
-    <row r="37" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+    </row>
+    <row r="37" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G37" s="10"/>
       <c r="J37" s="1"/>
-    </row>
-    <row r="38" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+    </row>
+    <row r="38" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G38" s="10"/>
       <c r="J38" s="1"/>
-    </row>
-    <row r="39" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+    </row>
+    <row r="39" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G39" s="10"/>
       <c r="J39" s="1"/>
-    </row>
-    <row r="40" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+    </row>
+    <row r="40" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G40" s="10"/>
       <c r="J40" s="1"/>
-    </row>
-    <row r="41" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+    </row>
+    <row r="41" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G41" s="10"/>
       <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="B3:E3"/>
-    <mergeCell ref="G3:O3"/>
-    <mergeCell ref="Q3:W3"/>
+    <mergeCell ref="S3:Y3"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B19:D19"/>
-    <mergeCell ref="G11:O11"/>
-    <mergeCell ref="M19:O19"/>
-    <mergeCell ref="Q19:W19"/>
-    <mergeCell ref="Q11:W11"/>
+    <mergeCell ref="G11:Q11"/>
+    <mergeCell ref="O19:Q19"/>
+    <mergeCell ref="S19:Y19"/>
+    <mergeCell ref="S11:Y11"/>
+    <mergeCell ref="I3:Q3"/>
   </mergeCells>
-  <conditionalFormatting sqref="S5:W9">
-    <cfRule type="colorScale" priority="14">
+  <conditionalFormatting sqref="U5:Y9">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1978,8 +2112,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y6:Z6 S5:W9">
-    <cfRule type="colorScale" priority="13">
+  <conditionalFormatting sqref="AA6:AB6 U5:Y9">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1990,8 +2124,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R5:R6 Y7:Z7">
-    <cfRule type="colorScale" priority="12">
+  <conditionalFormatting sqref="T5:T6 AA7:AB7">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2000,8 +2134,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R5:R9 Y7:Z7">
-    <cfRule type="colorScale" priority="11">
+  <conditionalFormatting sqref="T5:T9 AA7:AB7">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2010,8 +2144,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S21:W25">
-    <cfRule type="colorScale" priority="10">
+  <conditionalFormatting sqref="U21:Y25">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2022,8 +2156,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S21:W25">
-    <cfRule type="colorScale" priority="9">
+  <conditionalFormatting sqref="U21:Y25">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2034,8 +2168,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R21:R24">
-    <cfRule type="colorScale" priority="8">
+  <conditionalFormatting sqref="T21:T24">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2044,8 +2178,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R21:R25">
-    <cfRule type="colorScale" priority="7">
+  <conditionalFormatting sqref="T21:T25">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2054,7 +2188,31 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S5:W9 S21:W25 Y6:Z6">
+  <conditionalFormatting sqref="U5:Y9 U21:Y25 AA6:AB6">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U13:Y17">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U13:Y17">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -2066,8 +2224,28 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S13:W17">
+  <conditionalFormatting sqref="T13:T14">
     <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T13:T17">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U13:Y17">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2078,29 +2256,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S13:W17">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R13:R14">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R13:R17">
+  <conditionalFormatting sqref="AA7:AB7 T5:T9 T13:T17">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2110,7 +2266,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S13:W17">
+  <conditionalFormatting sqref="U5:Y9 U13:Y17 U21:Y25 AA6:AB6">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
'Network+Practical': obtained and added to report 'CNN_de' results
</commit_message>
<xml_diff>
--- a/02_network_and_practical/src/results/Fine_Tuning_Results.xlsx
+++ b/02_network_and_practical/src/results/Fine_Tuning_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniele\Documents\Programmazione\Github\Uni_NLP2022_Exam\02_network_and_practical\src\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A28B1C-0B7C-4860-B598-CF92AA823132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3915D5-68BE-4D8D-9E57-CCBBE90BD405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9015" yWindow="13125" windowWidth="19140" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="62">
   <si>
     <t>Language</t>
   </si>
@@ -186,9 +186,6 @@
     <t>1m 19s</t>
   </si>
   <si>
-    <t>1.6s</t>
-  </si>
-  <si>
     <t>Kernel Size</t>
   </si>
   <si>
@@ -202,6 +199,18 @@
   </si>
   <si>
     <t>2m 43s (on CPU)</t>
+  </si>
+  <si>
+    <t>2h 12m</t>
+  </si>
+  <si>
+    <t>1m 23s</t>
+  </si>
+  <si>
+    <t>1.66s</t>
+  </si>
+  <si>
+    <t>1.58s</t>
   </si>
 </sst>
 </file>
@@ -1027,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AB41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W47" sqref="W47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,7 +1505,7 @@
       <c r="P11" s="50"/>
       <c r="Q11" s="51"/>
       <c r="S11" s="49" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="T11" s="50"/>
       <c r="U11" s="50"/>
@@ -1531,13 +1540,13 @@
         <v>14</v>
       </c>
       <c r="K12" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="L12" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="L12" s="39" t="s">
+      <c r="M12" s="38" t="s">
         <v>55</v>
-      </c>
-      <c r="M12" s="38" t="s">
-        <v>56</v>
       </c>
       <c r="N12" s="38" t="s">
         <v>16</v>
@@ -1584,7 +1593,7 @@
         <v>52</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>4</v>
@@ -1645,9 +1654,15 @@
       <c r="B14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
+      <c r="C14" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>60</v>
+      </c>
       <c r="G14" s="6" t="s">
         <v>6</v>
       </c>
@@ -1853,7 +1868,7 @@
         <v>43</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
'Network+Practical': obtained 'CNN_it' res + redone all plots with same Y axis range
</commit_message>
<xml_diff>
--- a/02_network_and_practical/src/results/Fine_Tuning_Results.xlsx
+++ b/02_network_and_practical/src/results/Fine_Tuning_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniele\Documents\Programmazione\Github\Uni_NLP2022_Exam\02_network_and_practical\src\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3915D5-68BE-4D8D-9E57-CCBBE90BD405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9F71AA-05DA-4B2F-BA30-44B26A47B71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19260" yWindow="30" windowWidth="19140" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="62">
   <si>
     <t>Language</t>
   </si>
@@ -584,7 +584,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -746,6 +746,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1036,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AB41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W47" sqref="W47"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V30" sqref="V30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1183,7 +1192,7 @@
       <c r="N5" s="9">
         <v>1E-3</v>
       </c>
-      <c r="O5" s="9">
+      <c r="O5" s="55">
         <v>0</v>
       </c>
       <c r="P5" s="15">
@@ -1252,7 +1261,7 @@
       <c r="N6" s="12">
         <v>1E-3</v>
       </c>
-      <c r="O6" s="12">
+      <c r="O6" s="56">
         <v>0</v>
       </c>
       <c r="P6" s="16">
@@ -1283,7 +1292,7 @@
         <v>0.81459999999999999</v>
       </c>
       <c r="AA6" s="21">
-        <v>0.65</v>
+        <v>0.6</v>
       </c>
       <c r="AB6" s="22">
         <v>0.91500000000000004</v>
@@ -1321,7 +1330,7 @@
       <c r="N7" s="12">
         <v>1E-3</v>
       </c>
-      <c r="O7" s="12">
+      <c r="O7" s="56">
         <v>0</v>
       </c>
       <c r="P7" s="16">
@@ -1390,7 +1399,7 @@
       <c r="N8" s="12">
         <v>1E-3</v>
       </c>
-      <c r="O8" s="12">
+      <c r="O8" s="56">
         <v>0</v>
       </c>
       <c r="P8" s="16">
@@ -1452,7 +1461,7 @@
       <c r="N9" s="14">
         <v>1E-3</v>
       </c>
-      <c r="O9" s="14">
+      <c r="O9" s="57">
         <v>0</v>
       </c>
       <c r="P9" s="17">
@@ -1619,7 +1628,7 @@
       <c r="N13" s="9">
         <v>1E-3</v>
       </c>
-      <c r="O13" s="9">
+      <c r="O13" s="55">
         <v>0.1</v>
       </c>
       <c r="P13" s="15">
@@ -1672,31 +1681,65 @@
       <c r="I14" s="12">
         <v>4216</v>
       </c>
-      <c r="J14" s="12"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="16"/>
+      <c r="J14" s="12">
+        <v>2048</v>
+      </c>
+      <c r="K14" s="11">
+        <v>5</v>
+      </c>
+      <c r="L14" s="11">
+        <v>1</v>
+      </c>
+      <c r="M14" s="11">
+        <v>1</v>
+      </c>
+      <c r="N14" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="O14" s="56">
+        <v>0.1</v>
+      </c>
+      <c r="P14" s="16">
+        <v>31</v>
+      </c>
+      <c r="Q14" s="16">
+        <v>0.87309999999999999</v>
+      </c>
       <c r="S14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="T14" s="28"/>
-      <c r="U14" s="27"/>
-      <c r="V14" s="27"/>
-      <c r="W14" s="28"/>
-      <c r="X14" s="27"/>
-      <c r="Y14" s="27"/>
+      <c r="T14" s="28">
+        <v>0.72860000000000003</v>
+      </c>
+      <c r="U14" s="27">
+        <v>0.82079999999999997</v>
+      </c>
+      <c r="V14" s="27">
+        <v>0.82110000000000005</v>
+      </c>
+      <c r="W14" s="28">
+        <v>0.81459999999999999</v>
+      </c>
+      <c r="X14" s="27">
+        <v>0.83679999999999999</v>
+      </c>
+      <c r="Y14" s="27">
+        <v>0.81200000000000006</v>
+      </c>
     </row>
     <row r="15" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
+      <c r="C15" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>61</v>
+      </c>
       <c r="G15" s="6" t="s">
         <v>7</v>
       </c>
@@ -1706,23 +1749,51 @@
       <c r="I15" s="12">
         <v>4180</v>
       </c>
-      <c r="J15" s="12"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="16"/>
+      <c r="J15" s="12">
+        <v>2048</v>
+      </c>
+      <c r="K15" s="11">
+        <v>7</v>
+      </c>
+      <c r="L15" s="11">
+        <v>1</v>
+      </c>
+      <c r="M15" s="11">
+        <v>1</v>
+      </c>
+      <c r="N15" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="O15" s="56">
+        <v>0</v>
+      </c>
+      <c r="P15" s="16">
+        <v>20</v>
+      </c>
+      <c r="Q15" s="16">
+        <v>0.88929999999999998</v>
+      </c>
       <c r="S15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T15" s="28"/>
-      <c r="U15" s="27"/>
-      <c r="V15" s="27"/>
-      <c r="W15" s="27"/>
-      <c r="X15" s="28"/>
-      <c r="Y15" s="27"/>
+      <c r="T15" s="28">
+        <v>0.69189999999999996</v>
+      </c>
+      <c r="U15" s="27">
+        <v>0.85250000000000004</v>
+      </c>
+      <c r="V15" s="27">
+        <v>0.85170000000000001</v>
+      </c>
+      <c r="W15" s="27">
+        <v>0.86960000000000004</v>
+      </c>
+      <c r="X15" s="28">
+        <v>0.83420000000000005</v>
+      </c>
+      <c r="Y15" s="27">
+        <v>0.85119999999999996</v>
+      </c>
     </row>
     <row r="16" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
@@ -1745,7 +1816,7 @@
       <c r="L16" s="11"/>
       <c r="M16" s="11"/>
       <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
+      <c r="O16" s="56"/>
       <c r="P16" s="16"/>
       <c r="Q16" s="16"/>
       <c r="S16" s="6" t="s">
@@ -1779,7 +1850,7 @@
       <c r="L17" s="13"/>
       <c r="M17" s="13"/>
       <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
+      <c r="O17" s="57"/>
       <c r="P17" s="17"/>
       <c r="Q17" s="17"/>
       <c r="S17" s="7" t="s">

</xml_diff>

<commit_message>
'Network+Practical': obtained all results, updated images for report
</commit_message>
<xml_diff>
--- a/02_network_and_practical/src/results/Fine_Tuning_Results.xlsx
+++ b/02_network_and_practical/src/results/Fine_Tuning_Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniele\Documents\Programmazione\Github\Uni_NLP2022_Exam\02_network_and_practical\src\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9F71AA-05DA-4B2F-BA30-44B26A47B71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F9F28A-B108-4F50-BF48-147DAA767A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19260" yWindow="30" windowWidth="19140" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="68">
   <si>
     <t>Language</t>
   </si>
   <si>
-    <t>Training Time</t>
-  </si>
-  <si>
     <t>Mean Time per Model</t>
   </si>
   <si>
@@ -69,15 +66,9 @@
     <t>1m 11s</t>
   </si>
   <si>
-    <t>Embedding Dim</t>
-  </si>
-  <si>
     <t>Hidden Dim</t>
   </si>
   <si>
-    <t>Learning Rate</t>
-  </si>
-  <si>
     <t>Dropout</t>
   </si>
   <si>
@@ -198,19 +189,46 @@
     <t>[CNN] Test Set Results</t>
   </si>
   <si>
-    <t>2m 43s (on CPU)</t>
-  </si>
-  <si>
     <t>2h 12m</t>
   </si>
   <si>
     <t>1m 23s</t>
   </si>
   <si>
-    <t>1.66s</t>
-  </si>
-  <si>
-    <t>1.58s</t>
+    <t>Fine-Tuning Time</t>
+  </si>
+  <si>
+    <t>2m 43s</t>
+  </si>
+  <si>
+    <t>2h 10m</t>
+  </si>
+  <si>
+    <t>1m 21s</t>
+  </si>
+  <si>
+    <t>0.92</t>
+  </si>
+  <si>
+    <t>Emb. Dim</t>
+  </si>
+  <si>
+    <t>Learn. Rate</t>
+  </si>
+  <si>
+    <t>1h 58m</t>
+  </si>
+  <si>
+    <t>1,58s</t>
+  </si>
+  <si>
+    <t>1,66s</t>
+  </si>
+  <si>
+    <t>1,62s</t>
+  </si>
+  <si>
+    <t>1,48s</t>
   </si>
 </sst>
 </file>
@@ -247,7 +265,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,6 +332,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -584,7 +608,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -721,6 +745,18 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -746,15 +782,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1045,8 +1072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AB41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V30" sqref="V30"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="U33" sqref="U33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,9 +1083,9 @@
     <col min="3" max="3" width="23.7109375" style="1" customWidth="1"/>
     <col min="4" max="5" width="23.7109375" style="10" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="1"/>
-    <col min="7" max="7" width="16.7109375" style="1" customWidth="1"/>
-    <col min="8" max="12" width="16.7109375" style="10" customWidth="1"/>
-    <col min="13" max="16" width="16.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="1" customWidth="1"/>
+    <col min="8" max="12" width="12.7109375" style="10" customWidth="1"/>
+    <col min="13" max="16" width="12.7109375" style="1" customWidth="1"/>
     <col min="17" max="17" width="22.140625" style="1" customWidth="1"/>
     <col min="18" max="18" width="9.140625" style="1"/>
     <col min="19" max="19" width="12.7109375" style="1" customWidth="1"/>
@@ -1069,113 +1096,113 @@
   <sheetData>
     <row r="2" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:28" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="48"/>
+      <c r="B3" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="52"/>
       <c r="G3" s="10"/>
-      <c r="I3" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="48"/>
-      <c r="S3" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="T3" s="47"/>
-      <c r="U3" s="47"/>
-      <c r="V3" s="47"/>
-      <c r="W3" s="47"/>
-      <c r="X3" s="47"/>
-      <c r="Y3" s="48"/>
+      <c r="I3" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
+      <c r="Q3" s="52"/>
+      <c r="S3" s="50" t="s">
+        <v>37</v>
+      </c>
+      <c r="T3" s="51"/>
+      <c r="U3" s="51"/>
+      <c r="V3" s="51"/>
+      <c r="W3" s="51"/>
+      <c r="X3" s="51"/>
+      <c r="Y3" s="52"/>
     </row>
     <row r="4" spans="2:28" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="4" t="s">
         <v>2</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>3</v>
       </c>
       <c r="G4" s="10"/>
       <c r="I4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="J4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P4" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="P4" s="18" t="s">
-        <v>11</v>
-      </c>
       <c r="Q4" s="18" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="T4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="W4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="X4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>5</v>
-      </c>
       <c r="D5" s="9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5" s="10"/>
       <c r="I5" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J5" s="8">
         <v>64</v>
@@ -1192,17 +1219,17 @@
       <c r="N5" s="9">
         <v>1E-3</v>
       </c>
-      <c r="O5" s="55">
+      <c r="O5" s="46">
         <v>0</v>
       </c>
-      <c r="P5" s="15">
+      <c r="P5" s="9">
         <v>31</v>
       </c>
       <c r="Q5" s="15">
         <v>0.8488</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T5" s="26">
         <v>0.55610000000000004</v>
@@ -1223,28 +1250,28 @@
         <v>0.78590000000000004</v>
       </c>
       <c r="AA5" s="23" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="AB5" s="24" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>27</v>
-      </c>
       <c r="E6" s="12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G6" s="10"/>
       <c r="I6" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J6" s="11">
         <v>64</v>
@@ -1261,17 +1288,17 @@
       <c r="N6" s="12">
         <v>1E-3</v>
       </c>
-      <c r="O6" s="56">
+      <c r="O6" s="47">
         <v>0</v>
       </c>
-      <c r="P6" s="16">
+      <c r="P6" s="12">
         <v>42</v>
       </c>
       <c r="Q6" s="16">
         <v>0.77739999999999998</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T6" s="28">
         <v>0.92230000000000001</v>
@@ -1294,26 +1321,26 @@
       <c r="AA6" s="21">
         <v>0.6</v>
       </c>
-      <c r="AB6" s="22">
-        <v>0.91500000000000004</v>
+      <c r="AB6" s="22" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>28</v>
-      </c>
       <c r="E7" s="12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G7" s="10"/>
       <c r="I7" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J7" s="11">
         <v>64</v>
@@ -1330,17 +1357,17 @@
       <c r="N7" s="12">
         <v>1E-3</v>
       </c>
-      <c r="O7" s="56">
+      <c r="O7" s="47">
         <v>0</v>
       </c>
-      <c r="P7" s="16">
+      <c r="P7" s="12">
         <v>34</v>
       </c>
       <c r="Q7" s="16">
         <v>0.8538</v>
       </c>
       <c r="S7" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="T7" s="28">
         <v>0.54149999999999998</v>
@@ -1369,20 +1396,20 @@
     </row>
     <row r="8" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G8" s="10"/>
       <c r="I8" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J8" s="11">
         <v>64</v>
@@ -1399,17 +1426,17 @@
       <c r="N8" s="12">
         <v>1E-3</v>
       </c>
-      <c r="O8" s="56">
+      <c r="O8" s="47">
         <v>0</v>
       </c>
-      <c r="P8" s="16">
+      <c r="P8" s="12">
         <v>13</v>
       </c>
       <c r="Q8" s="16">
         <v>0.84619999999999995</v>
       </c>
       <c r="S8" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="T8" s="28">
         <v>0.6351</v>
@@ -1432,19 +1459,19 @@
     </row>
     <row r="9" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J9" s="13">
         <v>64</v>
@@ -1461,17 +1488,17 @@
       <c r="N9" s="14">
         <v>1E-3</v>
       </c>
-      <c r="O9" s="57">
+      <c r="O9" s="48">
         <v>0</v>
       </c>
-      <c r="P9" s="17">
+      <c r="P9" s="14">
         <v>48</v>
       </c>
       <c r="Q9" s="17">
         <v>0.84589999999999999</v>
       </c>
       <c r="S9" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T9" s="30">
         <v>0.92110000000000003</v>
@@ -1494,118 +1521,118 @@
     </row>
     <row r="10" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:28" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="49" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="51"/>
-      <c r="G11" s="49" t="s">
-        <v>50</v>
-      </c>
-      <c r="H11" s="50"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="50"/>
-      <c r="K11" s="50"/>
-      <c r="L11" s="50"/>
-      <c r="M11" s="50"/>
-      <c r="N11" s="50"/>
-      <c r="O11" s="50"/>
-      <c r="P11" s="50"/>
-      <c r="Q11" s="51"/>
-      <c r="S11" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="T11" s="50"/>
-      <c r="U11" s="50"/>
-      <c r="V11" s="50"/>
-      <c r="W11" s="50"/>
-      <c r="X11" s="50"/>
-      <c r="Y11" s="51"/>
+      <c r="B11" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="55"/>
+      <c r="G11" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="54"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="54"/>
+      <c r="N11" s="54"/>
+      <c r="O11" s="54"/>
+      <c r="P11" s="54"/>
+      <c r="Q11" s="55"/>
+      <c r="S11" s="53" t="s">
+        <v>53</v>
+      </c>
+      <c r="T11" s="54"/>
+      <c r="U11" s="54"/>
+      <c r="V11" s="54"/>
+      <c r="W11" s="54"/>
+      <c r="X11" s="54"/>
+      <c r="Y11" s="55"/>
     </row>
     <row r="12" spans="2:28" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="37" t="s">
         <v>0</v>
       </c>
       <c r="C12" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="38" t="s">
+      <c r="E12" s="39" t="s">
         <v>2</v>
-      </c>
-      <c r="E12" s="39" t="s">
-        <v>3</v>
       </c>
       <c r="G12" s="37" t="s">
         <v>0</v>
       </c>
       <c r="H12" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="K12" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="L12" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="M12" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="N12" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="O12" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="P12" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="J12" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="K12" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="L12" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="M12" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="N12" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="O12" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="P12" s="18" t="s">
-        <v>11</v>
-      </c>
       <c r="Q12" s="18" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="S12" s="37" t="s">
         <v>0</v>
       </c>
       <c r="T12" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="U12" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="V12" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="W12" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="U12" s="38" t="s">
+      <c r="X12" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="V12" s="38" t="s">
+      <c r="Y12" s="38" t="s">
         <v>20</v>
-      </c>
-      <c r="W12" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="X12" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y12" s="38" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H13" s="8">
         <v>64</v>
@@ -1628,17 +1655,17 @@
       <c r="N13" s="9">
         <v>1E-3</v>
       </c>
-      <c r="O13" s="55">
+      <c r="O13" s="46">
         <v>0.1</v>
       </c>
-      <c r="P13" s="15">
+      <c r="P13" s="9">
         <v>46</v>
       </c>
       <c r="Q13" s="15">
         <v>0.88739999999999997</v>
       </c>
       <c r="S13" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T13" s="26">
         <v>0.70850000000000002</v>
@@ -1661,19 +1688,19 @@
     </row>
     <row r="14" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H14" s="11">
         <v>64</v>
@@ -1696,17 +1723,17 @@
       <c r="N14" s="12">
         <v>1E-3</v>
       </c>
-      <c r="O14" s="56">
+      <c r="O14" s="47">
         <v>0.1</v>
       </c>
-      <c r="P14" s="16">
+      <c r="P14" s="12">
         <v>31</v>
       </c>
       <c r="Q14" s="16">
         <v>0.87309999999999999</v>
       </c>
       <c r="S14" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T14" s="28">
         <v>0.72860000000000003</v>
@@ -1729,19 +1756,19 @@
     </row>
     <row r="15" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H15" s="11">
         <v>64</v>
@@ -1764,17 +1791,17 @@
       <c r="N15" s="12">
         <v>1E-3</v>
       </c>
-      <c r="O15" s="56">
+      <c r="O15" s="47">
         <v>0</v>
       </c>
-      <c r="P15" s="16">
+      <c r="P15" s="12">
         <v>20</v>
       </c>
       <c r="Q15" s="16">
         <v>0.88929999999999998</v>
       </c>
       <c r="S15" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="T15" s="28">
         <v>0.69189999999999996</v>
@@ -1797,13 +1824,19 @@
     </row>
     <row r="16" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
+        <v>7</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>66</v>
+      </c>
       <c r="G16" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H16" s="11">
         <v>64</v>
@@ -1811,33 +1844,67 @@
       <c r="I16" s="12">
         <v>5255</v>
       </c>
-      <c r="J16" s="12"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="56"/>
-      <c r="P16" s="16"/>
-      <c r="Q16" s="16"/>
+      <c r="J16" s="12">
+        <v>2048</v>
+      </c>
+      <c r="K16" s="11">
+        <v>5</v>
+      </c>
+      <c r="L16" s="11">
+        <v>1</v>
+      </c>
+      <c r="M16" s="11">
+        <v>3</v>
+      </c>
+      <c r="N16" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="O16" s="47">
+        <v>0</v>
+      </c>
+      <c r="P16" s="12">
+        <v>12</v>
+      </c>
+      <c r="Q16" s="16">
+        <v>0.89290000000000003</v>
+      </c>
       <c r="S16" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="T16" s="28"/>
-      <c r="U16" s="27"/>
-      <c r="V16" s="27"/>
-      <c r="W16" s="28"/>
-      <c r="X16" s="27"/>
-      <c r="Y16" s="27"/>
+        <v>7</v>
+      </c>
+      <c r="T16" s="28">
+        <v>0.7137</v>
+      </c>
+      <c r="U16" s="27">
+        <v>0.83750000000000002</v>
+      </c>
+      <c r="V16" s="27">
+        <v>0.83809999999999996</v>
+      </c>
+      <c r="W16" s="28">
+        <v>0.82609999999999995</v>
+      </c>
+      <c r="X16" s="27">
+        <v>0.87370000000000003</v>
+      </c>
+      <c r="Y16" s="27">
+        <v>0.81459999999999999</v>
+      </c>
     </row>
     <row r="17" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
+        <v>8</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>67</v>
+      </c>
       <c r="G17" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H17" s="13">
         <v>64</v>
@@ -1845,59 +1912,87 @@
       <c r="I17" s="14">
         <v>4010</v>
       </c>
-      <c r="J17" s="14"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="57"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
+      <c r="J17" s="14">
+        <v>1024</v>
+      </c>
+      <c r="K17" s="13">
+        <v>7</v>
+      </c>
+      <c r="L17" s="13">
+        <v>1</v>
+      </c>
+      <c r="M17" s="13">
+        <v>1</v>
+      </c>
+      <c r="N17" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="O17" s="48">
+        <v>0.1</v>
+      </c>
+      <c r="P17" s="14">
+        <v>15</v>
+      </c>
+      <c r="Q17" s="17">
+        <v>0.86980000000000002</v>
+      </c>
       <c r="S17" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="T17" s="30"/>
-      <c r="U17" s="29"/>
-      <c r="V17" s="29"/>
-      <c r="W17" s="30"/>
-      <c r="X17" s="29"/>
-      <c r="Y17" s="29"/>
+        <v>8</v>
+      </c>
+      <c r="T17" s="30">
+        <v>0.71389999999999998</v>
+      </c>
+      <c r="U17" s="29">
+        <v>0.83079999999999998</v>
+      </c>
+      <c r="V17" s="29">
+        <v>0.82909999999999995</v>
+      </c>
+      <c r="W17" s="30">
+        <v>0.86960000000000004</v>
+      </c>
+      <c r="X17" s="29">
+        <v>0.83950000000000002</v>
+      </c>
+      <c r="Y17" s="29">
+        <v>0.77810000000000001</v>
+      </c>
     </row>
     <row r="18" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="2:25" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="52" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="53"/>
-      <c r="D19" s="54"/>
+      <c r="B19" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="57"/>
+      <c r="D19" s="58"/>
       <c r="G19" s="10"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
-      <c r="O19" s="52" t="s">
-        <v>46</v>
-      </c>
-      <c r="P19" s="53"/>
-      <c r="Q19" s="54"/>
-      <c r="S19" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="T19" s="53"/>
-      <c r="U19" s="53"/>
-      <c r="V19" s="53"/>
-      <c r="W19" s="53"/>
-      <c r="X19" s="53"/>
-      <c r="Y19" s="54"/>
+      <c r="O19" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="P19" s="57"/>
+      <c r="Q19" s="58"/>
+      <c r="S19" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="T19" s="57"/>
+      <c r="U19" s="57"/>
+      <c r="V19" s="57"/>
+      <c r="W19" s="57"/>
+      <c r="X19" s="57"/>
+      <c r="Y19" s="58"/>
     </row>
     <row r="20" spans="2:25" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="44" t="s">
         <v>0</v>
       </c>
       <c r="C20" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="45" t="s">
         <v>1</v>
-      </c>
-      <c r="D20" s="45" t="s">
-        <v>2</v>
       </c>
       <c r="G20" s="10"/>
       <c r="J20" s="1"/>
@@ -1907,46 +2002,46 @@
         <v>0</v>
       </c>
       <c r="P20" s="45" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q20" s="40" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="S20" s="44" t="s">
         <v>0</v>
       </c>
       <c r="T20" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="U20" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="V20" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="W20" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="U20" s="45" t="s">
+      <c r="X20" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="V20" s="45" t="s">
+      <c r="Y20" s="45" t="s">
         <v>20</v>
-      </c>
-      <c r="W20" s="45" t="s">
-        <v>21</v>
-      </c>
-      <c r="X20" s="45" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y20" s="45" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="21" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>57</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L21" s="1"/>
       <c r="O21" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P21" s="31">
         <v>1</v>
@@ -1955,10 +2050,10 @@
         <v>0.91120000000000001</v>
       </c>
       <c r="S21" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T21" s="41" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="U21" s="25">
         <v>0.87919999999999998</v>
@@ -1979,7 +2074,7 @@
     <row r="22" spans="2:25" x14ac:dyDescent="0.25">
       <c r="L22" s="1"/>
       <c r="O22" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P22" s="32">
         <v>1</v>
@@ -1988,10 +2083,10 @@
         <v>0.91214200000000001</v>
       </c>
       <c r="S22" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T22" s="42" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="U22" s="27">
         <v>0.87580000000000002</v>
@@ -2015,7 +2110,7 @@
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="O23" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P23" s="32">
         <v>1</v>
@@ -2024,10 +2119,10 @@
         <v>0.90961499999999995</v>
       </c>
       <c r="S23" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="T23" s="42" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="U23" s="27">
         <v>0.87749999999999995</v>
@@ -2051,7 +2146,7 @@
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="O24" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="P24" s="32">
         <v>1</v>
@@ -2060,10 +2155,10 @@
         <v>0.91226200000000002</v>
       </c>
       <c r="S24" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="T24" s="42" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="U24" s="27">
         <v>0.88</v>
@@ -2087,7 +2182,7 @@
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="O25" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P25" s="33">
         <v>1</v>
@@ -2096,10 +2191,10 @@
         <v>0.90903299999999998</v>
       </c>
       <c r="S25" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T25" s="43" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="U25" s="29">
         <v>0.88500000000000001</v>
@@ -2187,6 +2282,18 @@
     <mergeCell ref="I3:Q3"/>
   </mergeCells>
   <conditionalFormatting sqref="U5:Y9">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA6:AB6 U5:Y9">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -2198,19 +2305,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA6:AB6 U5:Y9">
+  <conditionalFormatting sqref="T5:T6 AA7:AB7">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T5:T6 AA7:AB7">
+  <conditionalFormatting sqref="T5:T9 AA7:AB7">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -2220,13 +2325,15 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T5:T9 AA7:AB7">
+  <conditionalFormatting sqref="U21:Y25">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -2242,8 +2349,28 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U21:Y25">
+  <conditionalFormatting sqref="T21:T24">
     <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T21:T25">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U5:Y9 U21:Y25 AA6:AB6">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2254,27 +2381,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T21:T24">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T21:T25">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U5:Y9 U21:Y25 AA6:AB6">
+  <conditionalFormatting sqref="U13:Y17">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -2298,19 +2405,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U13:Y17">
+  <conditionalFormatting sqref="T13:T14">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T13:T14">
+  <conditionalFormatting sqref="T13:T17">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -2320,18 +2425,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T13:T17">
+  <conditionalFormatting sqref="U13:Y17">
     <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U13:Y17">
-    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2343,7 +2438,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA7:AB7 T5:T9 T13:T17">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2353,6 +2448,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U5:Y9 U13:Y17 U21:Y25 AA6:AB6">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q5:Q9 Q13:Q17 Q21:Q25 AA6:AB6">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
'Network+Practical': completed first version of the report
</commit_message>
<xml_diff>
--- a/02_network_and_practical/src/results/Fine_Tuning_Results.xlsx
+++ b/02_network_and_practical/src/results/Fine_Tuning_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniele\Documents\Programmazione\Github\Uni_NLP2022_Exam\02_network_and_practical\src\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F9F28A-B108-4F50-BF48-147DAA767A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9685C82-9ECD-4D24-B308-817C4840B72E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,9 +39,6 @@
     <t>English</t>
   </si>
   <si>
-    <t>15h 44m (944m)</t>
-  </si>
-  <si>
     <t>German</t>
   </si>
   <si>
@@ -90,12 +87,6 @@
     <t>Accuracy [2]</t>
   </si>
   <si>
-    <t>16h 36m (996m)</t>
-  </si>
-  <si>
-    <t>14h 20m (860m)</t>
-  </si>
-  <si>
     <t>0h 59m</t>
   </si>
   <si>
@@ -120,15 +111,9 @@
     <t>MAX</t>
   </si>
   <si>
-    <t>15h 38m (938m)</t>
-  </si>
-  <si>
     <t>1m 10s</t>
   </si>
   <si>
-    <t>16h 12m (972m)</t>
-  </si>
-  <si>
     <t>1h 01m</t>
   </si>
   <si>
@@ -229,6 +214,21 @@
   </si>
   <si>
     <t>1,48s</t>
+  </si>
+  <si>
+    <t>15h 44m</t>
+  </si>
+  <si>
+    <t>16h 36m</t>
+  </si>
+  <si>
+    <t>14h 20m</t>
+  </si>
+  <si>
+    <t>15h 38m</t>
+  </si>
+  <si>
+    <t>16h 12m</t>
   </si>
 </sst>
 </file>
@@ -1072,8 +1072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AB41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="U33" sqref="U33"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1097,14 +1097,14 @@
     <row r="2" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:28" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="50" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C3" s="51"/>
       <c r="D3" s="51"/>
       <c r="E3" s="52"/>
       <c r="G3" s="10"/>
       <c r="I3" s="50" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="J3" s="51"/>
       <c r="K3" s="51"/>
@@ -1115,7 +1115,7 @@
       <c r="P3" s="51"/>
       <c r="Q3" s="52"/>
       <c r="S3" s="50" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="T3" s="51"/>
       <c r="U3" s="51"/>
@@ -1129,7 +1129,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>1</v>
@@ -1142,49 +1142,49 @@
         <v>0</v>
       </c>
       <c r="J4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="P4" s="49" t="s">
-        <v>10</v>
-      </c>
       <c r="Q4" s="18" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="T4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="U4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="X4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1192,13 +1192,13 @@
         <v>3</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5" s="10"/>
       <c r="I5" s="5" t="s">
@@ -1250,28 +1250,28 @@
         <v>0.78590000000000004</v>
       </c>
       <c r="AA5" s="23" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="AB5" s="24" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>24</v>
-      </c>
       <c r="E6" s="12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G6" s="10"/>
       <c r="I6" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J6" s="11">
         <v>64</v>
@@ -1298,7 +1298,7 @@
         <v>0.77739999999999998</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T6" s="28">
         <v>0.92230000000000001</v>
@@ -1322,25 +1322,25 @@
         <v>0.6</v>
       </c>
       <c r="AB6" s="22" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>25</v>
-      </c>
       <c r="E7" s="12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G7" s="10"/>
       <c r="I7" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J7" s="11">
         <v>64</v>
@@ -1367,7 +1367,7 @@
         <v>0.8538</v>
       </c>
       <c r="S7" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T7" s="28">
         <v>0.54149999999999998</v>
@@ -1396,20 +1396,20 @@
     </row>
     <row r="8" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G8" s="10"/>
       <c r="I8" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J8" s="11">
         <v>64</v>
@@ -1436,7 +1436,7 @@
         <v>0.84619999999999995</v>
       </c>
       <c r="S8" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="T8" s="28">
         <v>0.6351</v>
@@ -1459,19 +1459,19 @@
     </row>
     <row r="9" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J9" s="13">
         <v>64</v>
@@ -1498,7 +1498,7 @@
         <v>0.84589999999999999</v>
       </c>
       <c r="S9" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="T9" s="30">
         <v>0.92110000000000003</v>
@@ -1522,13 +1522,13 @@
     <row r="10" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:28" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="53" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C11" s="54"/>
       <c r="D11" s="54"/>
       <c r="E11" s="55"/>
       <c r="G11" s="53" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H11" s="54"/>
       <c r="I11" s="54"/>
@@ -1541,7 +1541,7 @@
       <c r="P11" s="54"/>
       <c r="Q11" s="55"/>
       <c r="S11" s="53" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="T11" s="54"/>
       <c r="U11" s="54"/>
@@ -1555,7 +1555,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D12" s="38" t="s">
         <v>1</v>
@@ -1567,55 +1567,55 @@
         <v>0</v>
       </c>
       <c r="H12" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="K12" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="L12" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="M12" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="N12" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="O12" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="P12" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="K12" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="L12" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="M12" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="N12" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="O12" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="P12" s="49" t="s">
-        <v>10</v>
-      </c>
       <c r="Q12" s="18" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="S12" s="37" t="s">
         <v>0</v>
       </c>
       <c r="T12" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="U12" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="U12" s="38" t="s">
+      <c r="V12" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="V12" s="38" t="s">
+      <c r="W12" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="W12" s="38" t="s">
+      <c r="X12" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="X12" s="38" t="s">
+      <c r="Y12" s="38" t="s">
         <v>19</v>
-      </c>
-      <c r="Y12" s="38" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="13" spans="2:28" x14ac:dyDescent="0.25">
@@ -1623,13 +1623,13 @@
         <v>3</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>3</v>
@@ -1688,19 +1688,19 @@
     </row>
     <row r="14" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H14" s="11">
         <v>64</v>
@@ -1733,7 +1733,7 @@
         <v>0.87309999999999999</v>
       </c>
       <c r="S14" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T14" s="28">
         <v>0.72860000000000003</v>
@@ -1756,19 +1756,19 @@
     </row>
     <row r="15" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H15" s="11">
         <v>64</v>
@@ -1801,7 +1801,7 @@
         <v>0.88929999999999998</v>
       </c>
       <c r="S15" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T15" s="28">
         <v>0.69189999999999996</v>
@@ -1824,19 +1824,19 @@
     </row>
     <row r="16" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H16" s="11">
         <v>64</v>
@@ -1869,7 +1869,7 @@
         <v>0.89290000000000003</v>
       </c>
       <c r="S16" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="T16" s="28">
         <v>0.7137</v>
@@ -1892,19 +1892,19 @@
     </row>
     <row r="17" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H17" s="13">
         <v>64</v>
@@ -1937,7 +1937,7 @@
         <v>0.86980000000000002</v>
       </c>
       <c r="S17" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="T17" s="30">
         <v>0.71389999999999998</v>
@@ -1961,7 +1961,7 @@
     <row r="18" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="2:25" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="56" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C19" s="57"/>
       <c r="D19" s="58"/>
@@ -1970,12 +1970,12 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="O19" s="56" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="P19" s="57"/>
       <c r="Q19" s="58"/>
       <c r="S19" s="56" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="T19" s="57"/>
       <c r="U19" s="57"/>
@@ -1989,7 +1989,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="45" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D20" s="45" t="s">
         <v>1</v>
@@ -2002,42 +2002,42 @@
         <v>0</v>
       </c>
       <c r="P20" s="45" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="Q20" s="40" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="S20" s="44" t="s">
         <v>0</v>
       </c>
       <c r="T20" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="U20" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="U20" s="45" t="s">
+      <c r="V20" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="V20" s="45" t="s">
+      <c r="W20" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="W20" s="45" t="s">
+      <c r="X20" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="X20" s="45" t="s">
+      <c r="Y20" s="45" t="s">
         <v>19</v>
-      </c>
-      <c r="Y20" s="45" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="21" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="L21" s="1"/>
       <c r="O21" s="5" t="s">
@@ -2053,7 +2053,7 @@
         <v>3</v>
       </c>
       <c r="T21" s="41" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="U21" s="25">
         <v>0.87919999999999998</v>
@@ -2074,7 +2074,7 @@
     <row r="22" spans="2:25" x14ac:dyDescent="0.25">
       <c r="L22" s="1"/>
       <c r="O22" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P22" s="32">
         <v>1</v>
@@ -2083,10 +2083,10 @@
         <v>0.91214200000000001</v>
       </c>
       <c r="S22" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T22" s="42" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="U22" s="27">
         <v>0.87580000000000002</v>
@@ -2110,7 +2110,7 @@
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="O23" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P23" s="32">
         <v>1</v>
@@ -2119,10 +2119,10 @@
         <v>0.90961499999999995</v>
       </c>
       <c r="S23" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T23" s="42" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="U23" s="27">
         <v>0.87749999999999995</v>
@@ -2146,7 +2146,7 @@
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="O24" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P24" s="32">
         <v>1</v>
@@ -2155,10 +2155,10 @@
         <v>0.91226200000000002</v>
       </c>
       <c r="S24" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="T24" s="42" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="U24" s="27">
         <v>0.88</v>
@@ -2182,7 +2182,7 @@
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="O25" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="P25" s="33">
         <v>1</v>
@@ -2191,10 +2191,10 @@
         <v>0.90903299999999998</v>
       </c>
       <c r="S25" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="T25" s="43" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="U25" s="29">
         <v>0.88500000000000001</v>

</xml_diff>